<commit_message>
Update Solid to transparent color converter.xlsx
</commit_message>
<xml_diff>
--- a/misc/Solid to transparent color converter.xlsx
+++ b/misc/Solid to transparent color converter.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\ElevenClock\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{430E78E0-0552-48DA-8508-03E69DB3EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87BD9D0-A9C1-4F74-8437-B48F09B937BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{654D62EF-35AB-4619-8AD6-AAECC88CD4CA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{654D62EF-35AB-4619-8AD6-AAECC88CD4CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Value</t>
   </si>
@@ -142,9 +141,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -156,6 +152,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +474,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,26 +501,26 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -547,7 +546,7 @@
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -560,26 +559,26 @@
     </row>
     <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="4" t="str">
         <f>DEC2HEX(C6)</f>
         <v>12</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>18</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>48</v>
       </c>
-      <c r="F6" s="5" t="str">
+      <c r="F6" s="4" t="str">
         <f>DEC2HEX(E6)</f>
         <v>30</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f>(E6-C6)+(E6-C6)*0.25+C6</f>
         <v>55.5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f>(E6-C6)+(E6-C6)*0.5+C6</f>
         <v>63</v>
       </c>
@@ -587,27 +586,27 @@
     </row>
     <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="4" t="str">
         <f>B6</f>
         <v>12</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f>C6</f>
         <v>18</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>54</v>
       </c>
-      <c r="F7" s="5" t="str">
+      <c r="F7" s="4" t="str">
         <f t="shared" ref="F7:F14" si="0">DEC2HEX(E7)</f>
         <v>36</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" ref="G7:G14" si="1">(E7-C7)+(E7-C7)*0.25+C7</f>
         <v>63</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" ref="H7:H14" si="2">(E7-C7)+(E7-C7)*0.5+C7</f>
         <v>72</v>
       </c>
@@ -615,27 +614,27 @@
     </row>
     <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="4" t="str">
         <f t="shared" ref="B8:B14" si="3">B7</f>
         <v>12</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f t="shared" ref="C8:C14" si="4">C7</f>
         <v>18</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>57</v>
       </c>
-      <c r="F8" s="5" t="str">
+      <c r="F8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>66.75</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="2"/>
         <v>76.5</v>
       </c>
@@ -643,27 +642,27 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="str">
+      <c r="B9" s="4" t="str">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>64</v>
       </c>
-      <c r="F9" s="5" t="str">
+      <c r="F9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>75.5</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
@@ -671,27 +670,27 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="4" t="str">
         <f>B9</f>
         <v>12</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>65</v>
       </c>
-      <c r="F10" s="5" t="str">
+      <c r="F10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>76.75</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="2"/>
         <v>88.5</v>
       </c>
@@ -699,27 +698,27 @@
     </row>
     <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="5" t="str">
+      <c r="B11" s="4" t="str">
         <f>B10</f>
         <v>12</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>69</v>
       </c>
-      <c r="F11" s="5" t="str">
+      <c r="F11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>81.75</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="2"/>
         <v>94.5</v>
       </c>
@@ -727,83 +726,83 @@
     </row>
     <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="5" t="str">
+      <c r="B12" s="4" t="str">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6">
+        <v>72</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>85.5</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="5" t="e">
+      <c r="F13" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G12" s="6" t="e">
+      <c r="G13" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H12" s="6" t="e">
+      <c r="H13" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5" t="str">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="str">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="5" t="e">
+      <c r="F14" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13" s="6" t="e">
+      <c r="G14" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="5">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="5" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G14" s="6" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="6" t="e">
+      <c r="H14" s="5" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Add mica effect to settings window
</commit_message>
<xml_diff>
--- a/misc/Solid to transparent color converter.xlsx
+++ b/misc/Solid to transparent color converter.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\ElevenClock\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87BD9D0-A9C1-4F74-8437-B48F09B937BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5705EE-9350-4FD6-92A1-C8B93DBDA8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{654D62EF-35AB-4619-8AD6-AAECC88CD4CA}"/>
   </bookViews>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Value</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Value (hex)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Bg Color (dec)</t>
@@ -175,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de l'Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Oficina">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +212,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Oficina">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Oficina">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,13 +468,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056769F1-16FF-4FB1-967D-BF9008F3E8FC}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -488,7 +485,7 @@
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -498,8 +495,9 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="8" t="s">
         <v>1</v>
@@ -511,8 +509,9 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -522,8 +521,9 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -533,14 +533,15 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
@@ -550,14 +551,17 @@
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="str">
         <f>DEC2HEX(C6)</f>
@@ -582,9 +586,13 @@
         <f>(E6-C6)+(E6-C6)*0.5+C6</f>
         <v>63</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <f>(E6-C6)+(E6-C6)*0.75+C6</f>
+        <v>70.5</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="str">
         <f>B6</f>
@@ -610,16 +618,20 @@
         <f t="shared" ref="H7:H14" si="2">(E7-C7)+(E7-C7)*0.5+C7</f>
         <v>72</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I7" s="5">
+        <f t="shared" ref="I7:I14" si="3">(E7-C7)+(E7-C7)*0.75+C7</f>
+        <v>81</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="str">
-        <f t="shared" ref="B8:B14" si="3">B7</f>
+        <f t="shared" ref="B8:B14" si="4">B7</f>
         <v>12</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:C14" si="4">C7</f>
+        <f t="shared" ref="C8:C14" si="5">C7</f>
         <v>18</v>
       </c>
       <c r="D8" s="3"/>
@@ -638,16 +650,20 @@
         <f t="shared" si="2"/>
         <v>76.5</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <f t="shared" si="3"/>
+        <v>86.25</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D9" s="3"/>
@@ -666,16 +682,20 @@
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I9" s="5">
+        <f t="shared" si="3"/>
+        <v>98.5</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="str">
         <f>B9</f>
         <v>12</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D10" s="3"/>
@@ -694,16 +714,20 @@
         <f t="shared" si="2"/>
         <v>88.5</v>
       </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I10" s="5">
+        <f t="shared" si="3"/>
+        <v>100.25</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="str">
         <f>B10</f>
         <v>12</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D11" s="3"/>
@@ -722,16 +746,20 @@
         <f t="shared" si="2"/>
         <v>94.5</v>
       </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I11" s="5">
+        <f t="shared" si="3"/>
+        <v>107.25</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D12" s="3"/>
@@ -750,65 +778,77 @@
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="I12" s="5">
+        <f t="shared" si="3"/>
+        <v>112.5</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6">
+        <v>112</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>135.5</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="I13" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G13" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+        <v>182.5</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="6">
+        <v>80</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="1"/>
+        <v>95.5</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G14" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>126.5</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -818,8 +858,9 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -829,8 +870,9 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -840,8 +882,9 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -851,8 +894,9 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -862,8 +906,9 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -873,6 +918,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1"/>

</xml_diff>